<commit_message>
Move test to tests directory and clean up
</commit_message>
<xml_diff>
--- a/tests/sample_questionnaire_1_question.xlsx
+++ b/tests/sample_questionnaire_1_question.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\QuestionnaireAgent_v2\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{57901B05-0FE0-4CE0-BDA6-E304A3891FEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E563E2B9-997E-4A1E-B0D0-E36129D0D34D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-5235" yWindow="-16297" windowWidth="28995" windowHeight="16395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,12 +36,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Please provide your company’s name</t>
-  </si>
-  <si>
-    <t>Please specify the year your company was founded</t>
   </si>
   <si>
     <t>Q#</t>
@@ -60,9 +57,6 @@
   </si>
   <si>
     <t>Documentation</t>
-  </si>
-  <si>
-    <t>Provide the contact details for your primary point of contact - name and email address</t>
   </si>
   <si>
     <t>not started</t>
@@ -692,7 +686,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E20" sqref="E20"/>
+      <selection pane="bottomRight" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -704,27 +698,27 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
       <c r="F1" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="3">
@@ -736,31 +730,19 @@
       <c r="E2" s="5"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="2" t="s">
-        <v>9</v>
-      </c>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" s="2"/>
       <c r="B3" s="2"/>
-      <c r="C3" s="3">
-        <v>2</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="4"/>
       <c r="E3" s="5"/>
       <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A4" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="A4" s="2"/>
       <c r="B4" s="2"/>
-      <c r="C4" s="3">
-        <v>3</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="4"/>
       <c r="E4" s="5"/>
       <c r="F4" s="2"/>
     </row>

</xml_diff>